<commit_message>
Comparativas DG y GII
</commit_message>
<xml_diff>
--- a/raw_alumnos.xlsx
+++ b/raw_alumnos.xlsx
@@ -152,7 +152,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -162,6 +162,7 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -476,16 +477,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:BX30"/>
+  <dimension ref="A1:CH30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="BQ1" workbookViewId="0">
+      <selection activeCell="CD14" sqref="CD14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="90.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
@@ -714,8 +717,38 @@
       <c r="BX1" s="2">
         <v>5</v>
       </c>
+      <c r="BY1" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ1" s="5">
+        <v>4</v>
+      </c>
+      <c r="CA1" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB1" s="5">
+        <v>4</v>
+      </c>
+      <c r="CC1" s="5">
+        <v>4</v>
+      </c>
+      <c r="CD1" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE1" s="5">
+        <v>4</v>
+      </c>
+      <c r="CF1" s="5">
+        <v>4</v>
+      </c>
+      <c r="CG1" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH1" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="2" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="3" t="s">
         <v>1</v>
       </c>
@@ -944,8 +977,38 @@
       <c r="BX2" s="3">
         <v>0</v>
       </c>
+      <c r="BY2" s="5">
+        <v>4</v>
+      </c>
+      <c r="BZ2" s="5">
+        <v>4</v>
+      </c>
+      <c r="CA2" s="5">
+        <v>4</v>
+      </c>
+      <c r="CB2" s="5">
+        <v>4</v>
+      </c>
+      <c r="CC2" s="5">
+        <v>3</v>
+      </c>
+      <c r="CD2" s="5">
+        <v>5</v>
+      </c>
+      <c r="CE2" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF2" s="5">
+        <v>4</v>
+      </c>
+      <c r="CG2" s="5">
+        <v>1</v>
+      </c>
+      <c r="CH2" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="3" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="3" t="s">
         <v>2</v>
       </c>
@@ -1174,8 +1237,38 @@
       <c r="BX3" s="2">
         <v>4</v>
       </c>
+      <c r="BY3" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ3" s="5">
+        <v>4</v>
+      </c>
+      <c r="CA3" s="5">
+        <v>2</v>
+      </c>
+      <c r="CB3" s="5">
+        <v>3</v>
+      </c>
+      <c r="CC3" s="5">
+        <v>5</v>
+      </c>
+      <c r="CD3" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE3" s="5">
+        <v>5</v>
+      </c>
+      <c r="CF3" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG3" s="5">
+        <v>4</v>
+      </c>
+      <c r="CH3" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="4" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
         <v>3</v>
       </c>
@@ -1404,8 +1497,38 @@
       <c r="BX4" s="2">
         <v>2</v>
       </c>
+      <c r="BY4" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ4" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA4" s="5">
+        <v>2</v>
+      </c>
+      <c r="CB4" s="5">
+        <v>3</v>
+      </c>
+      <c r="CC4" s="5">
+        <v>4</v>
+      </c>
+      <c r="CD4" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE4" s="5">
+        <v>3</v>
+      </c>
+      <c r="CF4" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG4" s="5">
+        <v>1</v>
+      </c>
+      <c r="CH4" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="5" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
         <v>4</v>
       </c>
@@ -1634,8 +1757,38 @@
       <c r="BX5" s="2">
         <v>1</v>
       </c>
+      <c r="BY5" s="5">
+        <v>4</v>
+      </c>
+      <c r="BZ5" s="5">
+        <v>4</v>
+      </c>
+      <c r="CA5" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB5" s="5">
+        <v>4</v>
+      </c>
+      <c r="CC5" s="5">
+        <v>5</v>
+      </c>
+      <c r="CD5" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE5" s="5">
+        <v>3</v>
+      </c>
+      <c r="CF5" s="5">
+        <v>5</v>
+      </c>
+      <c r="CG5" s="5">
+        <v>4</v>
+      </c>
+      <c r="CH5" s="5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="6" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
         <v>5</v>
       </c>
@@ -1864,8 +2017,38 @@
       <c r="BX6" s="3">
         <v>0</v>
       </c>
+      <c r="BY6" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ6" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA6" s="5">
+        <v>4</v>
+      </c>
+      <c r="CB6" s="5">
+        <v>4</v>
+      </c>
+      <c r="CC6" s="5">
+        <v>4</v>
+      </c>
+      <c r="CD6" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE6" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF6" s="5">
+        <v>4</v>
+      </c>
+      <c r="CG6" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH6" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="7" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
         <v>6</v>
       </c>
@@ -2094,8 +2277,38 @@
       <c r="BX7" s="2">
         <v>4</v>
       </c>
+      <c r="BY7" s="5">
+        <v>4</v>
+      </c>
+      <c r="BZ7" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA7" s="5">
+        <v>2</v>
+      </c>
+      <c r="CB7" s="5">
+        <v>2</v>
+      </c>
+      <c r="CC7" s="5">
+        <v>5</v>
+      </c>
+      <c r="CD7" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE7" s="5">
+        <v>4</v>
+      </c>
+      <c r="CF7" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG7" s="5">
+        <v>2</v>
+      </c>
+      <c r="CH7" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="8" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
         <v>7</v>
       </c>
@@ -2324,8 +2537,38 @@
       <c r="BX8" s="2">
         <v>3</v>
       </c>
+      <c r="BY8" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ8" s="5">
+        <v>4</v>
+      </c>
+      <c r="CA8" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB8" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC8" s="5">
+        <v>5</v>
+      </c>
+      <c r="CD8" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE8" s="5">
+        <v>4</v>
+      </c>
+      <c r="CF8" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG8" s="5">
+        <v>2</v>
+      </c>
+      <c r="CH8" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="9" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="3" t="s">
         <v>8</v>
       </c>
@@ -2554,8 +2797,38 @@
       <c r="BX9" s="2">
         <v>4</v>
       </c>
+      <c r="BY9" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ9" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA9" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB9" s="5">
+        <v>3</v>
+      </c>
+      <c r="CC9" s="5">
+        <v>5</v>
+      </c>
+      <c r="CD9" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE9" s="5">
+        <v>5</v>
+      </c>
+      <c r="CF9" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG9" s="5">
+        <v>2</v>
+      </c>
+      <c r="CH9" s="5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="10" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="3" t="s">
         <v>9</v>
       </c>
@@ -2784,8 +3057,38 @@
       <c r="BX10" s="2">
         <v>2</v>
       </c>
+      <c r="BY10" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ10" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA10" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB10" s="5">
+        <v>2</v>
+      </c>
+      <c r="CC10" s="5">
+        <v>4</v>
+      </c>
+      <c r="CD10" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE10" s="5">
+        <v>2</v>
+      </c>
+      <c r="CF10" s="5">
+        <v>2</v>
+      </c>
+      <c r="CG10" s="5">
+        <v>1</v>
+      </c>
+      <c r="CH10" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="11" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="3" t="s">
         <v>10</v>
       </c>
@@ -3014,8 +3317,38 @@
       <c r="BX11" s="2">
         <v>0</v>
       </c>
+      <c r="BY11" s="5">
+        <v>4</v>
+      </c>
+      <c r="BZ11" s="5">
+        <v>4</v>
+      </c>
+      <c r="CA11" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB11" s="5">
+        <v>5</v>
+      </c>
+      <c r="CC11" s="5">
+        <v>3</v>
+      </c>
+      <c r="CD11" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE11" s="5">
+        <v>3</v>
+      </c>
+      <c r="CF11" s="5">
+        <v>2</v>
+      </c>
+      <c r="CG11" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH11" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="12" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="3" t="s">
         <v>11</v>
       </c>
@@ -3244,8 +3577,38 @@
       <c r="BX12" s="2">
         <v>0</v>
       </c>
+      <c r="BY12" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ12" s="5">
+        <v>4</v>
+      </c>
+      <c r="CA12" s="5">
+        <v>2</v>
+      </c>
+      <c r="CB12" s="5">
+        <v>3</v>
+      </c>
+      <c r="CC12" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD12" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE12" s="5">
+        <v>1</v>
+      </c>
+      <c r="CF12" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG12" s="5">
+        <v>2</v>
+      </c>
+      <c r="CH12" s="5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="13" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="3" t="s">
         <v>12</v>
       </c>
@@ -3474,8 +3837,38 @@
       <c r="BX13" s="2">
         <v>4</v>
       </c>
+      <c r="BY13" s="5">
+        <v>4</v>
+      </c>
+      <c r="BZ13" s="5">
+        <v>5</v>
+      </c>
+      <c r="CA13" s="5">
+        <v>4</v>
+      </c>
+      <c r="CB13" s="5">
+        <v>4</v>
+      </c>
+      <c r="CC13" s="5">
+        <v>5</v>
+      </c>
+      <c r="CD13" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE13" s="5">
+        <v>4</v>
+      </c>
+      <c r="CF13" s="5">
+        <v>5</v>
+      </c>
+      <c r="CG13" s="5">
+        <v>5</v>
+      </c>
+      <c r="CH13" s="5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="14" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>13</v>
       </c>
@@ -3704,8 +4097,38 @@
       <c r="BX14" s="2">
         <v>0</v>
       </c>
+      <c r="BY14" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ14" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA14" s="5">
+        <v>4</v>
+      </c>
+      <c r="CB14" s="5">
+        <v>3</v>
+      </c>
+      <c r="CC14" s="5">
+        <v>3</v>
+      </c>
+      <c r="CD14" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE14" s="5">
+        <v>3</v>
+      </c>
+      <c r="CF14" s="5">
+        <v>4</v>
+      </c>
+      <c r="CG14" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH14" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="15" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="3" t="s">
         <v>14</v>
       </c>
@@ -3934,8 +4357,38 @@
       <c r="BX15" s="2">
         <v>4</v>
       </c>
+      <c r="BY15" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ15" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA15" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB15" s="5">
+        <v>3</v>
+      </c>
+      <c r="CC15" s="5">
+        <v>4</v>
+      </c>
+      <c r="CD15" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE15" s="5">
+        <v>4</v>
+      </c>
+      <c r="CF15" s="5">
+        <v>4</v>
+      </c>
+      <c r="CG15" s="5">
+        <v>4</v>
+      </c>
+      <c r="CH15" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="16" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="3" t="s">
         <v>15</v>
       </c>
@@ -4164,8 +4617,38 @@
       <c r="BX16" s="2">
         <v>2</v>
       </c>
+      <c r="BY16" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ16" s="5">
+        <v>4</v>
+      </c>
+      <c r="CA16" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB16" s="5">
+        <v>2</v>
+      </c>
+      <c r="CC16" s="5">
+        <v>2</v>
+      </c>
+      <c r="CD16" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE16" s="5">
+        <v>5</v>
+      </c>
+      <c r="CF16" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG16" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH16" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="17" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>16</v>
       </c>
@@ -4394,8 +4877,38 @@
       <c r="BX17" s="2">
         <v>4</v>
       </c>
+      <c r="BY17" s="5">
+        <v>4</v>
+      </c>
+      <c r="BZ17" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA17" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB17" s="5">
+        <v>3</v>
+      </c>
+      <c r="CC17" s="5">
+        <v>4</v>
+      </c>
+      <c r="CD17" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE17" s="5">
+        <v>5</v>
+      </c>
+      <c r="CF17" s="5">
+        <v>4</v>
+      </c>
+      <c r="CG17" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH17" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="18" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="3" t="s">
         <v>17</v>
       </c>
@@ -4624,8 +5137,38 @@
       <c r="BX18" s="3">
         <v>0</v>
       </c>
+      <c r="BY18" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ18" s="5">
+        <v>1</v>
+      </c>
+      <c r="CA18" s="5">
+        <v>2</v>
+      </c>
+      <c r="CB18" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC18" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD18" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE18" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF18" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG18" s="5">
+        <v>1</v>
+      </c>
+      <c r="CH18" s="5">
+        <v>0</v>
+      </c>
     </row>
-    <row r="19" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="3" t="s">
         <v>18</v>
       </c>
@@ -4854,8 +5397,38 @@
       <c r="BX19" s="2">
         <v>3</v>
       </c>
+      <c r="BY19" s="5">
+        <v>1</v>
+      </c>
+      <c r="BZ19" s="5">
+        <v>1</v>
+      </c>
+      <c r="CA19" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB19" s="5">
+        <v>1</v>
+      </c>
+      <c r="CC19" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD19" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE19" s="5">
+        <v>2</v>
+      </c>
+      <c r="CF19" s="5">
+        <v>2</v>
+      </c>
+      <c r="CG19" s="5">
+        <v>2</v>
+      </c>
+      <c r="CH19" s="5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="20" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="3" t="s">
         <v>19</v>
       </c>
@@ -5084,8 +5657,38 @@
       <c r="BX20" s="2">
         <v>1</v>
       </c>
+      <c r="BY20" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ20" s="5">
+        <v>2</v>
+      </c>
+      <c r="CA20" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB20" s="5">
+        <v>2</v>
+      </c>
+      <c r="CC20" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD20" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE20" s="5">
+        <v>1</v>
+      </c>
+      <c r="CF20" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG20" s="5">
+        <v>1</v>
+      </c>
+      <c r="CH20" s="5">
+        <v>1</v>
+      </c>
     </row>
-    <row r="21" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="3" t="s">
         <v>20</v>
       </c>
@@ -5314,8 +5917,38 @@
       <c r="BX21" s="2">
         <v>0</v>
       </c>
+      <c r="BY21" s="5">
+        <v>2</v>
+      </c>
+      <c r="BZ21" s="5">
+        <v>2</v>
+      </c>
+      <c r="CA21" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB21" s="5">
+        <v>3</v>
+      </c>
+      <c r="CC21" s="5">
+        <v>2</v>
+      </c>
+      <c r="CD21" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE21" s="5">
+        <v>3</v>
+      </c>
+      <c r="CF21" s="5">
+        <v>1</v>
+      </c>
+      <c r="CG21" s="5">
+        <v>1</v>
+      </c>
+      <c r="CH21" s="5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="22" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="3" t="s">
         <v>21</v>
       </c>
@@ -5544,8 +6177,38 @@
       <c r="BX22" s="2">
         <v>0</v>
       </c>
+      <c r="BY22" s="5">
+        <v>2</v>
+      </c>
+      <c r="BZ22" s="5">
+        <v>1</v>
+      </c>
+      <c r="CA22" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB22" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC22" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD22" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE22" s="5">
+        <v>1</v>
+      </c>
+      <c r="CF22" s="5">
+        <v>2</v>
+      </c>
+      <c r="CG22" s="5">
+        <v>0</v>
+      </c>
+      <c r="CH22" s="5">
+        <v>2</v>
+      </c>
     </row>
-    <row r="23" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="3" t="s">
         <v>22</v>
       </c>
@@ -5774,8 +6437,38 @@
       <c r="BX23" s="2">
         <v>0</v>
       </c>
+      <c r="BY23" s="5">
+        <v>2</v>
+      </c>
+      <c r="BZ23" s="5">
+        <v>1</v>
+      </c>
+      <c r="CA23" s="5">
+        <v>2</v>
+      </c>
+      <c r="CB23" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC23" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD23" s="5">
+        <v>3</v>
+      </c>
+      <c r="CE23" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF23" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG23" s="5">
+        <v>0</v>
+      </c>
+      <c r="CH23" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="24" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="3" t="s">
         <v>23</v>
       </c>
@@ -6004,8 +6697,38 @@
       <c r="BX24" s="2">
         <v>5</v>
       </c>
+      <c r="BY24" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ24" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA24" s="5">
+        <v>4</v>
+      </c>
+      <c r="CB24" s="5">
+        <v>1</v>
+      </c>
+      <c r="CC24" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD24" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE24" s="5">
+        <v>1</v>
+      </c>
+      <c r="CF24" s="5">
+        <v>2</v>
+      </c>
+      <c r="CG24" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH24" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="25" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="3" t="s">
         <v>24</v>
       </c>
@@ -6234,8 +6957,38 @@
       <c r="BX25" s="3">
         <v>0</v>
       </c>
+      <c r="BY25" s="5">
+        <v>1</v>
+      </c>
+      <c r="BZ25" s="5">
+        <v>1</v>
+      </c>
+      <c r="CA25" s="5">
+        <v>2</v>
+      </c>
+      <c r="CB25" s="5">
+        <v>1</v>
+      </c>
+      <c r="CC25" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD25" s="5">
+        <v>2</v>
+      </c>
+      <c r="CE25" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF25" s="5">
+        <v>4</v>
+      </c>
+      <c r="CG25" s="5">
+        <v>0</v>
+      </c>
+      <c r="CH25" s="5">
+        <v>4</v>
+      </c>
     </row>
-    <row r="26" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>25</v>
       </c>
@@ -6464,8 +7217,38 @@
       <c r="BX26" s="2">
         <v>2</v>
       </c>
+      <c r="BY26" s="5">
+        <v>2</v>
+      </c>
+      <c r="BZ26" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA26" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB26" s="5">
+        <v>5</v>
+      </c>
+      <c r="CC26" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD26" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE26" s="5">
+        <v>1</v>
+      </c>
+      <c r="CF26" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG26" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH26" s="5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="27" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="3" t="s">
         <v>26</v>
       </c>
@@ -6694,8 +7477,38 @@
       <c r="BX27" s="2">
         <v>3</v>
       </c>
+      <c r="BY27" s="5">
+        <v>4</v>
+      </c>
+      <c r="BZ27" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA27" s="5">
+        <v>2</v>
+      </c>
+      <c r="CB27" s="5">
+        <v>4</v>
+      </c>
+      <c r="CC27" s="5">
+        <v>1</v>
+      </c>
+      <c r="CD27" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE27" s="5">
+        <v>3</v>
+      </c>
+      <c r="CF27" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG27" s="5">
+        <v>4</v>
+      </c>
+      <c r="CH27" s="5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="28" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="3" t="s">
         <v>27</v>
       </c>
@@ -6924,8 +7737,38 @@
       <c r="BX28" s="2">
         <v>0</v>
       </c>
+      <c r="BY28" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ28" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA28" s="5">
+        <v>3</v>
+      </c>
+      <c r="CB28" s="5">
+        <v>4</v>
+      </c>
+      <c r="CC28" s="5">
+        <v>2</v>
+      </c>
+      <c r="CD28" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE28" s="5">
+        <v>5</v>
+      </c>
+      <c r="CF28" s="5">
+        <v>3</v>
+      </c>
+      <c r="CG28" s="5">
+        <v>4</v>
+      </c>
+      <c r="CH28" s="5">
+        <v>5</v>
+      </c>
     </row>
-    <row r="29" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>28</v>
       </c>
@@ -7154,8 +7997,38 @@
       <c r="BX29" s="2">
         <v>3</v>
       </c>
+      <c r="BY29" s="5">
+        <v>3</v>
+      </c>
+      <c r="BZ29" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA29" s="5">
+        <v>4</v>
+      </c>
+      <c r="CB29" s="5">
+        <v>2</v>
+      </c>
+      <c r="CC29" s="5">
+        <v>3</v>
+      </c>
+      <c r="CD29" s="5">
+        <v>4</v>
+      </c>
+      <c r="CE29" s="5">
+        <v>2</v>
+      </c>
+      <c r="CF29" s="5">
+        <v>2</v>
+      </c>
+      <c r="CG29" s="5">
+        <v>3</v>
+      </c>
+      <c r="CH29" s="5">
+        <v>3</v>
+      </c>
     </row>
-    <row r="30" spans="1:76" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:86" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="3" t="s">
         <v>29</v>
       </c>
@@ -7382,6 +8255,36 @@
         <v>5</v>
       </c>
       <c r="BX30" s="3">
+        <v>0</v>
+      </c>
+      <c r="BY30" s="5">
+        <v>0</v>
+      </c>
+      <c r="BZ30" s="5">
+        <v>3</v>
+      </c>
+      <c r="CA30" s="5">
+        <v>1</v>
+      </c>
+      <c r="CB30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CC30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CD30" s="5">
+        <v>5</v>
+      </c>
+      <c r="CE30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CF30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CG30" s="5">
+        <v>0</v>
+      </c>
+      <c r="CH30" s="5">
         <v>0</v>
       </c>
     </row>

</xml_diff>